<commit_message>
Added inverse time mode arc test - edits to the rest
</commit_message>
<xml_diff>
--- a/tests/005-Arcs/ArcTestWorkbook-150425.xlsx
+++ b/tests/005-Arcs/ArcTestWorkbook-150425.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="200" windowWidth="19140" windowHeight="24820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18900" windowHeight="16640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scratch" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
     <sheet name="ArcTests-Exceptions" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -1293,15 +1293,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1554,16 +1550,16 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Accent1 - 20%" xfId="3" builtinId="30"/>
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
     <cellStyle name="Accent4" xfId="4" builtinId="41"/>
-    <cellStyle name="Accent4 - 20%" xfId="5" builtinId="42"/>
-    <cellStyle name="Accent5 - 20%" xfId="6" builtinId="46"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1888,14 +1884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="125" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="14" customWidth="1"/>
@@ -2390,7 +2386,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2398,14 +2394,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="E156" sqref="E156"/>
+    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="E235" sqref="E235"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
@@ -4293,7 +4289,7 @@
       </c>
     </row>
     <row r="164" spans="1:7">
-      <c r="A164" s="35" t="s">
+      <c r="A164" s="38" t="s">
         <v>333</v>
       </c>
       <c r="B164" s="29"/>
@@ -4568,7 +4564,7 @@
       </c>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="35" t="s">
+      <c r="A186" s="38" t="s">
         <v>332</v>
       </c>
       <c r="B186" s="29"/>
@@ -6742,7 +6738,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -6750,14 +6746,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
@@ -7359,7 +7355,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7367,16 +7363,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Moving some tests up
</commit_message>
<xml_diff>
--- a/tests/005-Arcs/ArcTestWorkbook-150425.xlsx
+++ b/tests/005-Arcs/ArcTestWorkbook-150425.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18900" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="15700" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scratch" sheetId="1" r:id="rId1"/>
     <sheet name="ArcTests-Baseline" sheetId="2" r:id="rId2"/>
     <sheet name="ArcTests-Exceptions" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="circle points" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="398">
   <si>
     <t>G2 I5 J4 X5 Y5</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1340,15 +1340,25 @@
   <si>
     <t>Radius</t>
   </si>
+  <si>
+    <t>scale radius</t>
+  </si>
+  <si>
+    <t>translate X</t>
+  </si>
+  <si>
+    <t>translate Y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1449,6 +1459,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1514,7 +1530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1556,8 +1572,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1634,8 +1754,13 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="145">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
     <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
@@ -1658,6 +1783,58 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -1676,6 +1853,58 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2005,18 +2234,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J62"/>
+  <dimension ref="B1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="A71" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:XFD92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="14" customWidth="1"/>
-    <col min="3" max="5" width="9" style="14" customWidth="1"/>
-    <col min="6" max="7" width="9" customWidth="1"/>
+    <col min="3" max="5" width="9.33203125" style="14" customWidth="1"/>
+    <col min="6" max="11" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
@@ -2686,7 +2915,7 @@
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:11">
       <c r="B49" s="14" t="s">
         <v>384</v>
       </c>
@@ -2711,7 +2940,7 @@
         <v>1.22514845490862E-16</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:11">
       <c r="B50" s="14" t="s">
         <v>385</v>
       </c>
@@ -2736,7 +2965,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:11">
       <c r="B51" s="14" t="s">
         <v>386</v>
       </c>
@@ -2756,7 +2985,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:11">
       <c r="B52" s="14" t="s">
         <v>387</v>
       </c>
@@ -2776,7 +3005,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="2:11">
       <c r="B53" s="14" t="s">
         <v>388</v>
       </c>
@@ -2796,7 +3025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:11">
       <c r="B54" s="14" t="s">
         <v>389</v>
       </c>
@@ -2816,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:11">
       <c r="B55" s="14" t="s">
         <v>392</v>
       </c>
@@ -2841,7 +3070,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:11">
       <c r="B56" s="14" t="s">
         <v>393</v>
       </c>
@@ -2866,7 +3095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:11">
       <c r="B57" s="14" t="s">
         <v>394</v>
       </c>
@@ -2891,7 +3120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:11">
       <c r="B58" s="14" t="s">
         <v>390</v>
       </c>
@@ -2916,7 +3145,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:11">
       <c r="B59" s="14" t="s">
         <v>391</v>
       </c>
@@ -2941,10 +3170,1040 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="2:11">
+      <c r="B62" s="14" t="s">
+        <v>382</v>
+      </c>
       <c r="C62" s="14">
-        <f>SQRT((67.67-75)^2 + (67.67-50)^2)</f>
-        <v>19.130023523247431</v>
+        <v>0.1</v>
+      </c>
+      <c r="D62" s="14">
+        <v>45</v>
+      </c>
+      <c r="E62" s="14">
+        <v>90</v>
+      </c>
+      <c r="F62" s="14">
+        <v>135</v>
+      </c>
+      <c r="G62" s="14">
+        <v>180</v>
+      </c>
+      <c r="H62">
+        <f>G62+45</f>
+        <v>225</v>
+      </c>
+      <c r="I62" s="14">
+        <v>270</v>
+      </c>
+      <c r="J62">
+        <f>I62+45</f>
+        <v>315</v>
+      </c>
+      <c r="K62" s="14">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="B63" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C63" s="17">
+        <f>PI()*C62/180</f>
+        <v>1.7453292519943296E-3</v>
+      </c>
+      <c r="D63" s="17">
+        <f>PI()*D62/180</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E63" s="17">
+        <f t="shared" ref="E63:K63" si="10">PI()*E62/180</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F63" s="17">
+        <f t="shared" si="10"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="G63" s="17">
+        <f t="shared" si="10"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="H63" s="17">
+        <f t="shared" si="10"/>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="I63" s="17">
+        <f t="shared" si="10"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="J63" s="17">
+        <f t="shared" si="10"/>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="K63" s="17">
+        <f t="shared" si="10"/>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="B64" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C64" s="17">
+        <f>SIN(C63)</f>
+        <v>1.7453283658983088E-3</v>
+      </c>
+      <c r="D64" s="17">
+        <f>SIN(D63)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E64" s="17">
+        <f t="shared" ref="E64:G64" si="11">SIN(E63)</f>
+        <v>1</v>
+      </c>
+      <c r="F64" s="17">
+        <f t="shared" si="11"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="G64" s="17">
+        <f t="shared" si="11"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="H64" s="17">
+        <f t="shared" ref="H64:K64" si="12">SIN(H63)</f>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I64" s="17">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="J64" s="17">
+        <f t="shared" si="12"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="K64" s="17">
+        <f t="shared" si="12"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11">
+      <c r="B65" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="C65" s="17">
+        <f>COS(C63)</f>
+        <v>0.99999847691328769</v>
+      </c>
+      <c r="D65" s="17">
+        <f>COS(D63)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E65" s="17">
+        <f t="shared" ref="E65:G65" si="13">COS(E63)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="F65" s="17">
+        <f t="shared" si="13"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="G65" s="17">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
+      <c r="H65" s="17">
+        <f t="shared" ref="H65:K65" si="14">COS(H63)</f>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="I65" s="17">
+        <f t="shared" si="14"/>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="J65" s="17">
+        <f t="shared" si="14"/>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="K65" s="17">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11">
+      <c r="B66" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C66" s="14">
+        <v>0</v>
+      </c>
+      <c r="D66" s="14">
+        <f>C66</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="14">
+        <f t="shared" ref="E66:K66" si="15">D66</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="H66" s="14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="C67" s="14">
+        <v>0</v>
+      </c>
+      <c r="D67" s="14">
+        <f>C67</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="14">
+        <f t="shared" ref="E67:K67" si="16">D67</f>
+        <v>0</v>
+      </c>
+      <c r="F67" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H67" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I67" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K67" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="B68" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C68" s="14">
+        <v>25</v>
+      </c>
+      <c r="D68" s="14">
+        <f>C68</f>
+        <v>25</v>
+      </c>
+      <c r="E68" s="14">
+        <f t="shared" ref="E68:K68" si="17">D68</f>
+        <v>25</v>
+      </c>
+      <c r="F68" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="G68" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="H68" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="I68" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="J68" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="K68" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11">
+      <c r="B69" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C69" s="14">
+        <v>0</v>
+      </c>
+      <c r="D69" s="14">
+        <f>C69</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="14">
+        <f t="shared" ref="E69:K69" si="18">D69</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H69" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I69" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K69" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11">
+      <c r="B70" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C70" s="14">
+        <f>C66+C68</f>
+        <v>25</v>
+      </c>
+      <c r="D70" s="14">
+        <f>C70</f>
+        <v>25</v>
+      </c>
+      <c r="E70" s="14">
+        <f t="shared" ref="E70:K70" si="19">D70</f>
+        <v>25</v>
+      </c>
+      <c r="F70" s="14">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="G70" s="14">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="H70" s="14">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="I70" s="14">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="J70" s="14">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="K70" s="14">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11">
+      <c r="B71" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C71" s="14">
+        <f>C67+C69</f>
+        <v>0</v>
+      </c>
+      <c r="D71" s="14">
+        <f>C71</f>
+        <v>0</v>
+      </c>
+      <c r="E71" s="14">
+        <f t="shared" ref="E71:K71" si="20">D71</f>
+        <v>0</v>
+      </c>
+      <c r="F71" s="14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H71" s="14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I71" s="14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J71" s="14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K71" s="14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11">
+      <c r="B72" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C72" s="14">
+        <f>SQRT(C68^2+C69^2)</f>
+        <v>25</v>
+      </c>
+      <c r="D72" s="14">
+        <f>C72</f>
+        <v>25</v>
+      </c>
+      <c r="E72" s="14">
+        <f t="shared" ref="E72:K72" si="21">D72</f>
+        <v>25</v>
+      </c>
+      <c r="F72" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="G72" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="H72" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="I72" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="J72" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="K72" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11">
+      <c r="B73" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C73" s="14">
+        <f>C70-C64*C72</f>
+        <v>24.956366790852542</v>
+      </c>
+      <c r="D73" s="14">
+        <f>D70-D64*D72</f>
+        <v>7.3223304703363148</v>
+      </c>
+      <c r="E73" s="14">
+        <f t="shared" ref="E73:G73" si="22">E70-E64*E72</f>
+        <v>0</v>
+      </c>
+      <c r="F73" s="14">
+        <f t="shared" si="22"/>
+        <v>7.3223304703363112</v>
+      </c>
+      <c r="G73" s="14">
+        <f t="shared" si="22"/>
+        <v>24.999999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11">
+      <c r="B74" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C74" s="14">
+        <f>C71+C65*C72</f>
+        <v>24.999961922832192</v>
+      </c>
+      <c r="D74" s="14">
+        <f>D71+D65*D72</f>
+        <v>17.677669529663689</v>
+      </c>
+      <c r="E74" s="14">
+        <f t="shared" ref="E74:G74" si="23">E71+E65*E72</f>
+        <v>1.531435568635775E-15</v>
+      </c>
+      <c r="F74" s="14">
+        <f t="shared" si="23"/>
+        <v>-17.677669529663685</v>
+      </c>
+      <c r="G74" s="14">
+        <f t="shared" si="23"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11">
+      <c r="B76" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="C76" s="14">
+        <v>1</v>
+      </c>
+      <c r="D76" s="14">
+        <v>45</v>
+      </c>
+      <c r="E76" s="14">
+        <v>90</v>
+      </c>
+      <c r="F76" s="14">
+        <v>135</v>
+      </c>
+      <c r="G76" s="14">
+        <v>180</v>
+      </c>
+      <c r="H76">
+        <f>G76+45</f>
+        <v>225</v>
+      </c>
+      <c r="I76" s="14">
+        <v>270</v>
+      </c>
+      <c r="J76">
+        <f>I76+45</f>
+        <v>315</v>
+      </c>
+      <c r="K76" s="14">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C77" s="17">
+        <f>PI()*C76/180</f>
+        <v>1.7453292519943295E-2</v>
+      </c>
+      <c r="D77" s="17">
+        <f>PI()*D76/180</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E77" s="17">
+        <f t="shared" ref="E77:K77" si="24">PI()*E76/180</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F77" s="17">
+        <f t="shared" si="24"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="G77" s="17">
+        <f t="shared" si="24"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="H77" s="17">
+        <f t="shared" si="24"/>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="I77" s="17">
+        <f t="shared" si="24"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="J77" s="17">
+        <f t="shared" si="24"/>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="K77" s="17">
+        <f t="shared" si="24"/>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C78" s="17">
+        <f>SIN(C77)</f>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="D78" s="17">
+        <f>SIN(D77)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E78" s="17">
+        <f t="shared" ref="E78:K78" si="25">SIN(E77)</f>
+        <v>1</v>
+      </c>
+      <c r="F78" s="17">
+        <f t="shared" si="25"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="G78" s="17">
+        <f t="shared" si="25"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="H78" s="17">
+        <f t="shared" si="25"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I78" s="17">
+        <f t="shared" si="25"/>
+        <v>-1</v>
+      </c>
+      <c r="J78" s="17">
+        <f t="shared" si="25"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="K78" s="17">
+        <f t="shared" si="25"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11">
+      <c r="B79" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="C79" s="17">
+        <f>COS(C77)</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="D79" s="17">
+        <f>COS(D77)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E79" s="17">
+        <f t="shared" ref="E79:K79" si="26">COS(E77)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="F79" s="17">
+        <f t="shared" si="26"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="G79" s="17">
+        <f t="shared" si="26"/>
+        <v>-1</v>
+      </c>
+      <c r="H79" s="17">
+        <f t="shared" si="26"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="I79" s="17">
+        <f t="shared" si="26"/>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="J79" s="17">
+        <f t="shared" si="26"/>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="K79" s="17">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11">
+      <c r="B80" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C80" s="14">
+        <v>1</v>
+      </c>
+      <c r="D80" s="14">
+        <f>C80</f>
+        <v>1</v>
+      </c>
+      <c r="E80" s="14">
+        <f t="shared" ref="E80:K80" si="27">D80</f>
+        <v>1</v>
+      </c>
+      <c r="F80" s="14">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="G80" s="14">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="H80" s="14">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="I80" s="14">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="J80" s="14">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="K80" s="14">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11">
+      <c r="B81" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="C81" s="14">
+        <v>0</v>
+      </c>
+      <c r="D81" s="14">
+        <f>C81</f>
+        <v>0</v>
+      </c>
+      <c r="E81" s="14">
+        <f t="shared" ref="E81:K81" si="28">D81</f>
+        <v>0</v>
+      </c>
+      <c r="F81" s="14">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="G81" s="14">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H81" s="14">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I81" s="14">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J81" s="14">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K81" s="14">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11">
+      <c r="B82" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C82" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D82" s="14">
+        <f>C82</f>
+        <v>-1</v>
+      </c>
+      <c r="E82" s="14">
+        <f t="shared" ref="E82:K82" si="29">D82</f>
+        <v>-1</v>
+      </c>
+      <c r="F82" s="14">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="G82" s="14">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="H82" s="14">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="I82" s="14">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="J82" s="14">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="K82" s="14">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11">
+      <c r="B83" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C83" s="14">
+        <v>0</v>
+      </c>
+      <c r="D83" s="14">
+        <f>C83</f>
+        <v>0</v>
+      </c>
+      <c r="E83" s="14">
+        <f t="shared" ref="E83:K83" si="30">D83</f>
+        <v>0</v>
+      </c>
+      <c r="F83" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="G83" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="H83" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="I83" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J83" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="K83" s="14">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11">
+      <c r="B84" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C84" s="14">
+        <f>C80+C82</f>
+        <v>0</v>
+      </c>
+      <c r="D84" s="14">
+        <f>C84</f>
+        <v>0</v>
+      </c>
+      <c r="E84" s="14">
+        <f t="shared" ref="E84:K84" si="31">D84</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="14">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="G84" s="14">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="H84" s="14">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="I84" s="14">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="J84" s="14">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="K84" s="14">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11">
+      <c r="B85" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C85" s="14">
+        <f>C81+C83</f>
+        <v>0</v>
+      </c>
+      <c r="D85" s="14">
+        <f>C85</f>
+        <v>0</v>
+      </c>
+      <c r="E85" s="14">
+        <f t="shared" ref="E85:K85" si="32">D85</f>
+        <v>0</v>
+      </c>
+      <c r="F85" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="G85" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="H85" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="I85" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J85" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="K85" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11">
+      <c r="B86" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C86" s="14">
+        <f>SQRT(C82^2+C83^2)</f>
+        <v>1</v>
+      </c>
+      <c r="D86" s="14">
+        <f>C86</f>
+        <v>1</v>
+      </c>
+      <c r="E86" s="14">
+        <f t="shared" ref="E86:K86" si="33">D86</f>
+        <v>1</v>
+      </c>
+      <c r="F86" s="14">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="G86" s="14">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="H86" s="14">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="I86" s="14">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="J86" s="14">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="K86" s="14">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11">
+      <c r="B87" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C87" s="40">
+        <f>C86*C79</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="D87" s="40">
+        <f t="shared" ref="D87:K87" si="34">D86*D79</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E87" s="40">
+        <f t="shared" si="34"/>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="F87" s="40">
+        <f t="shared" si="34"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="G87" s="40">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="H87" s="40">
+        <f t="shared" si="34"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="I87" s="40">
+        <f t="shared" si="34"/>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="J87" s="40">
+        <f t="shared" si="34"/>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="K87" s="40">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11">
+      <c r="B88" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C88" s="40">
+        <f>C86*C78</f>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="D88" s="40">
+        <f t="shared" ref="D88:K88" si="35">D86*D78</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E88" s="40">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="F88" s="40">
+        <f t="shared" si="35"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="G88" s="40">
+        <f t="shared" si="35"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="H88" s="40">
+        <f t="shared" si="35"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I88" s="40">
+        <f t="shared" si="35"/>
+        <v>-1</v>
+      </c>
+      <c r="J88" s="40">
+        <f t="shared" si="35"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="K88" s="40">
+        <f t="shared" si="35"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11">
+      <c r="B90" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C90" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11">
+      <c r="B91" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="C91" s="14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11">
+      <c r="B92" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="C92" s="14">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -7933,16 +9192,1530 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetData>
+    <row r="1" spans="2:18">
+      <c r="B1" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" s="19">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19">
+        <v>45</v>
+      </c>
+      <c r="E1" s="19">
+        <v>89</v>
+      </c>
+      <c r="F1" s="19">
+        <v>90</v>
+      </c>
+      <c r="G1" s="19">
+        <v>91</v>
+      </c>
+      <c r="H1" s="19">
+        <v>135</v>
+      </c>
+      <c r="I1" s="19">
+        <v>179</v>
+      </c>
+      <c r="J1" s="19">
+        <v>180</v>
+      </c>
+      <c r="K1" s="19">
+        <v>181</v>
+      </c>
+      <c r="L1" s="41">
+        <f>J1+45</f>
+        <v>225</v>
+      </c>
+      <c r="M1" s="19">
+        <v>269</v>
+      </c>
+      <c r="N1" s="19">
+        <v>270</v>
+      </c>
+      <c r="O1" s="19">
+        <v>271</v>
+      </c>
+      <c r="P1" s="41">
+        <f>N1+45</f>
+        <v>315</v>
+      </c>
+      <c r="Q1" s="19">
+        <v>359</v>
+      </c>
+      <c r="R1" s="19">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18">
+      <c r="B2" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="17">
+        <f>PI()*C1/180</f>
+        <v>1.7453292519943295E-2</v>
+      </c>
+      <c r="D2" s="17">
+        <f>PI()*D1/180</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E2" s="17">
+        <f t="shared" ref="E2:R2" si="0">PI()*E1/180</f>
+        <v>1.5533430342749535</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="G2" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5882496193148399</v>
+      </c>
+      <c r="H2" s="17">
+        <f t="shared" si="0"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="I2" s="17">
+        <f t="shared" si="0"/>
+        <v>3.12413936106985</v>
+      </c>
+      <c r="J2" s="17">
+        <f t="shared" si="0"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K2" s="17">
+        <f t="shared" si="0"/>
+        <v>3.1590459461097362</v>
+      </c>
+      <c r="L2" s="17">
+        <f t="shared" si="0"/>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="M2" s="17">
+        <f t="shared" si="0"/>
+        <v>4.6949356878647466</v>
+      </c>
+      <c r="N2" s="17">
+        <f t="shared" si="0"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="O2" s="17">
+        <f t="shared" si="0"/>
+        <v>4.7298422729046328</v>
+      </c>
+      <c r="P2" s="17">
+        <f t="shared" si="0"/>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="Q2" s="17">
+        <f t="shared" si="0"/>
+        <v>6.2657320146596422</v>
+      </c>
+      <c r="R2" s="17">
+        <f t="shared" si="0"/>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C3" s="17">
+        <f>SIN(C2)</f>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="D3" s="17">
+        <f>SIN(D2)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E3" s="17">
+        <f t="shared" ref="E3:R3" si="1">SIN(E2)</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" si="1"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="H3" s="17">
+        <f t="shared" si="1"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="I3" s="17">
+        <f t="shared" si="1"/>
+        <v>1.7452406437283439E-2</v>
+      </c>
+      <c r="J3" s="17">
+        <f t="shared" si="1"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="K3" s="17">
+        <f t="shared" si="1"/>
+        <v>-1.7452406437283192E-2</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" si="1"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="M3" s="17">
+        <f t="shared" si="1"/>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="N3" s="17">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="O3" s="17">
+        <f t="shared" si="1"/>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="P3" s="17">
+        <f t="shared" si="1"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="Q3" s="17">
+        <f t="shared" si="1"/>
+        <v>-1.7452406437284448E-2</v>
+      </c>
+      <c r="R3" s="17">
+        <f t="shared" si="1"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" s="17">
+        <f>COS(C2)</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="D4" s="17">
+        <f>COS(D2)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E4" s="17">
+        <f t="shared" ref="E4:R4" si="2">COS(E2)</f>
+        <v>1.7452406437283376E-2</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" si="2"/>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.7452406437283477E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I4" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="J4" s="17">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="K4" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="L4" s="17">
+        <f t="shared" si="2"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="M4" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.7452406437283498E-2</v>
+      </c>
+      <c r="N4" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="O4" s="17">
+        <f t="shared" si="2"/>
+        <v>1.745240643728313E-2</v>
+      </c>
+      <c r="P4" s="17">
+        <f t="shared" si="2"/>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="Q4" s="17">
+        <f t="shared" si="2"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="R4" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" ref="E5:R5" si="3">D5</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="B6" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <f>C6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" ref="E6:R6" si="4">D6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" s="19">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="14">
+        <f>C7</f>
+        <v>-1</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" ref="E7:R7" si="5">D7</f>
+        <v>-1</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <f>C8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" ref="E8:R8" si="6">D8</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C9" s="19">
+        <f>C5+C7</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <f>C9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" ref="E9:R9" si="7">D9</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10" s="19">
+        <f>C6+C8</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <f>C10</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" ref="E10:R10" si="8">D10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C11" s="19">
+        <f>SQRT(C7^2+C8^2)</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <f>C11</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" ref="E11:R11" si="9">D11</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" s="40">
+        <f>C11*C4</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="D12" s="40">
+        <f t="shared" ref="D12:R12" si="10">D11*D4</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E12" s="40">
+        <f t="shared" ref="E12" si="11">E11*E4</f>
+        <v>1.7452406437283376E-2</v>
+      </c>
+      <c r="F12" s="40">
+        <f t="shared" ref="F12" si="12">F11*F4</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="G12" s="40">
+        <f t="shared" ref="G12" si="13">G11*G4</f>
+        <v>-1.7452406437283477E-2</v>
+      </c>
+      <c r="H12" s="40">
+        <f t="shared" ref="H12" si="14">H11*H4</f>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I12" s="40">
+        <f t="shared" ref="I12" si="15">I11*I4</f>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="J12" s="40">
+        <f t="shared" ref="J12" si="16">J11*J4</f>
+        <v>-1</v>
+      </c>
+      <c r="K12" s="40">
+        <f t="shared" ref="K12" si="17">K11*K4</f>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="L12" s="40">
+        <f t="shared" ref="L12" si="18">L11*L4</f>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="M12" s="40">
+        <f t="shared" ref="M12" si="19">M11*M4</f>
+        <v>-1.7452406437283498E-2</v>
+      </c>
+      <c r="N12" s="40">
+        <f t="shared" ref="N12" si="20">N11*N4</f>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="O12" s="40">
+        <f t="shared" ref="O12" si="21">O11*O4</f>
+        <v>1.745240643728313E-2</v>
+      </c>
+      <c r="P12" s="40">
+        <f t="shared" ref="P12" si="22">P11*P4</f>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="Q12" s="40">
+        <f t="shared" ref="Q12" si="23">Q11*Q4</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="R12" s="40">
+        <f t="shared" ref="R12" si="24">R11*R4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="B13" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C13" s="40">
+        <f>C11*C3</f>
+        <v>1.7452406437283512E-2</v>
+      </c>
+      <c r="D13" s="40">
+        <f t="shared" ref="D13:R13" si="25">D11*D3</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E13" s="40">
+        <f t="shared" ref="E13:R13" si="26">E11*E3</f>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="F13" s="40">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="40">
+        <f t="shared" si="26"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="H13" s="40">
+        <f t="shared" si="26"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="I13" s="40">
+        <f t="shared" si="26"/>
+        <v>1.7452406437283439E-2</v>
+      </c>
+      <c r="J13" s="40">
+        <f t="shared" si="26"/>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="K13" s="40">
+        <f t="shared" si="26"/>
+        <v>-1.7452406437283192E-2</v>
+      </c>
+      <c r="L13" s="40">
+        <f t="shared" si="26"/>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="M13" s="40">
+        <f t="shared" si="26"/>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="N13" s="40">
+        <f t="shared" si="26"/>
+        <v>-1</v>
+      </c>
+      <c r="O13" s="40">
+        <f t="shared" si="26"/>
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="P13" s="40">
+        <f t="shared" si="26"/>
+        <v>-0.70710678118654768</v>
+      </c>
+      <c r="Q13" s="40">
+        <f t="shared" si="26"/>
+        <v>-1.7452406437284448E-2</v>
+      </c>
+      <c r="R13" s="40">
+        <f t="shared" si="26"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="B15" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C15" s="19">
+        <v>25</v>
+      </c>
+      <c r="D15" s="14">
+        <f>C15</f>
+        <v>25</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" ref="E15:R15" si="27">D15</f>
+        <v>25</v>
+      </c>
+      <c r="F15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="G15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="H15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="I15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="J15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="K15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="N15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="O15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="P15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="Q15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="R15" s="14">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="C16" s="19">
+        <v>50</v>
+      </c>
+      <c r="D16" s="14">
+        <f t="shared" ref="D16:R17" si="28">C16</f>
+        <v>50</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="G16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="I16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="N16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="O16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="P16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="Q16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="R16" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="C17" s="19">
+        <v>50</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="G17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="I17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="K17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="M17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="N17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="O17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="P17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="Q17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+      <c r="R17" s="14">
+        <f t="shared" si="28"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C18">
+        <f>C11*C15+C16</f>
+        <v>75</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:R18" si="29">D11*D15+D16</f>
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="29"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="C19">
+        <f>C11*C15+C17</f>
+        <v>75</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:R19" si="30">D11*D15+D17</f>
+        <v>75</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C20">
+        <f>C7*C15</f>
+        <v>-25</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:R20" si="31">D7*D15</f>
+        <v>-25</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="31"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18">
+      <c r="B21" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C21">
+        <f>C8*C15</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:R21" si="32">D8*D15</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18">
+      <c r="B22" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C22" s="42">
+        <f>C15*C12+C16</f>
+        <v>74.996192378909782</v>
+      </c>
+      <c r="D22" s="42">
+        <f t="shared" ref="D22:R22" si="33">D15*D12+D16</f>
+        <v>67.677669529663689</v>
+      </c>
+      <c r="E22" s="42">
+        <f t="shared" si="33"/>
+        <v>50.436310160932088</v>
+      </c>
+      <c r="F22" s="42">
+        <f t="shared" si="33"/>
+        <v>50</v>
+      </c>
+      <c r="G22" s="42">
+        <f t="shared" si="33"/>
+        <v>49.563689839067912</v>
+      </c>
+      <c r="H22" s="42">
+        <f t="shared" si="33"/>
+        <v>32.322330470336311</v>
+      </c>
+      <c r="I22" s="42">
+        <f t="shared" si="33"/>
+        <v>25.003807621090218</v>
+      </c>
+      <c r="J22" s="42">
+        <f t="shared" si="33"/>
+        <v>25</v>
+      </c>
+      <c r="K22" s="42">
+        <f t="shared" si="33"/>
+        <v>25.003807621090218</v>
+      </c>
+      <c r="L22" s="42">
+        <f t="shared" si="33"/>
+        <v>32.322330470336311</v>
+      </c>
+      <c r="M22" s="42">
+        <f t="shared" si="33"/>
+        <v>49.563689839067912</v>
+      </c>
+      <c r="N22" s="42">
+        <f t="shared" si="33"/>
+        <v>49.999999999999993</v>
+      </c>
+      <c r="O22" s="42">
+        <f t="shared" si="33"/>
+        <v>50.436310160932081</v>
+      </c>
+      <c r="P22" s="42">
+        <f t="shared" si="33"/>
+        <v>67.677669529663689</v>
+      </c>
+      <c r="Q22" s="42">
+        <f t="shared" si="33"/>
+        <v>74.996192378909782</v>
+      </c>
+      <c r="R22" s="42">
+        <f t="shared" si="33"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="B23" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C23" s="42">
+        <f>C15*C13+C17</f>
+        <v>50.436310160932088</v>
+      </c>
+      <c r="D23" s="42">
+        <f t="shared" ref="D23:R23" si="34">D15*D13+D17</f>
+        <v>67.677669529663689</v>
+      </c>
+      <c r="E23" s="42">
+        <f t="shared" si="34"/>
+        <v>74.996192378909782</v>
+      </c>
+      <c r="F23" s="42">
+        <f t="shared" si="34"/>
+        <v>75</v>
+      </c>
+      <c r="G23" s="42">
+        <f t="shared" si="34"/>
+        <v>74.996192378909782</v>
+      </c>
+      <c r="H23" s="42">
+        <f t="shared" si="34"/>
+        <v>67.677669529663689</v>
+      </c>
+      <c r="I23" s="42">
+        <f t="shared" si="34"/>
+        <v>50.436310160932088</v>
+      </c>
+      <c r="J23" s="42">
+        <f t="shared" si="34"/>
+        <v>50</v>
+      </c>
+      <c r="K23" s="42">
+        <f t="shared" si="34"/>
+        <v>49.563689839067919</v>
+      </c>
+      <c r="L23" s="42">
+        <f t="shared" si="34"/>
+        <v>32.322330470336311</v>
+      </c>
+      <c r="M23" s="42">
+        <f t="shared" si="34"/>
+        <v>25.003807621090218</v>
+      </c>
+      <c r="N23" s="42">
+        <f t="shared" si="34"/>
+        <v>25</v>
+      </c>
+      <c r="O23" s="42">
+        <f t="shared" si="34"/>
+        <v>25.003807621090218</v>
+      </c>
+      <c r="P23" s="42">
+        <f t="shared" si="34"/>
+        <v>32.322330470336311</v>
+      </c>
+      <c r="Q23" s="42">
+        <f t="shared" si="34"/>
+        <v>49.563689839067891</v>
+      </c>
+      <c r="R23" s="42">
+        <f t="shared" si="34"/>
+        <v>49.999999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="62" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>